<commit_message>
added code for extra timetable
</commit_message>
<xml_diff>
--- a/Lab_timetable.xlsx
+++ b/Lab_timetable.xlsx
@@ -518,12 +518,12 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                 </t>
+          <t xml:space="preserve">JAVA (Lab - BCA Lab by MN, SR, VKR, MAN) in 3CM                      </t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                 </t>
+          <t xml:space="preserve">JAVA (Lab - BCA Lab by MN, SR, VKR, MAN) in 3CM                      </t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -572,12 +572,12 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                 </t>
+          <t xml:space="preserve">JAVA (Lab - BCA Lab by KNS, RES, VKR, MAN) in 3CS                    </t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                 </t>
+          <t xml:space="preserve">JAVA (Lab - BCA Lab by KNS, RES, VKR, MAN) in 3CS                    </t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -626,47 +626,47 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                    </t>
+          <t xml:space="preserve">PY (Lab - BCA Lab by KNS, NR, TM, KR, VA) in 3BCA A </t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                    </t>
+          <t xml:space="preserve">PY (Lab - BCA Lab by KNS, NR, TM, KR, VA) in 3BCA A </t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                    </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>OOP (Lab - BCA Lab by KNS, LJ) in 1BCA B</t>
+          <t xml:space="preserve">OOP (Lab - BCA Lab by KNS, LJ) in 1BCA B            </t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>OOP (Lab - BCA Lab by KNS, LJ) in 1BCA B</t>
+          <t xml:space="preserve">OOP (Lab - BCA Lab by KNS, LJ) in 1BCA B            </t>
         </is>
       </c>
       <c r="G5" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                    </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="H5" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                    </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="I5" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                    </t>
+          <t>OOP (Lab - BCA Lab by CHA, RV, SD, SH, SA) in 1BCA A</t>
         </is>
       </c>
       <c r="J5" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                    </t>
+          <t>OOP (Lab - BCA Lab by CHA, RV, SD, SH, SA) in 1BCA A</t>
         </is>
       </c>
     </row>
@@ -678,47 +678,47 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">PY (Lab - BCA Lab by HU, RA, APR, RES, KR) in 3BCA B </t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">PY (Lab - BCA Lab by HU, RA, APR, RES, KR) in 3BCA B </t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="G6" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="H6" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="I6" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t>PSD (Lab - BCA Lab by CHA, FHP, NR, SD, SH) in 1BCA A</t>
         </is>
       </c>
       <c r="J6" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t>PSD (Lab - BCA Lab by CHA, FHP, NR, SD, SH) in 1BCA A</t>
         </is>
       </c>
     </row>
@@ -730,47 +730,47 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t>MA (Lab - BCA Lab by NR, CYN, SD, SH, MAN) in 3BCA A</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t>MA (Lab - BCA Lab by NR, CYN, SD, SH, MAN) in 3BCA A</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>MA (Lab - BCA Lab by VKR) in 5BCA A</t>
+          <t xml:space="preserve">MA (Lab - BCA Lab by VKR) in 5BCA A                 </t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>MA (Lab - BCA Lab by VKR) in 5BCA A</t>
+          <t xml:space="preserve">MA (Lab - BCA Lab by VKR) in 5BCA A                 </t>
         </is>
       </c>
       <c r="G7" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="H7" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="I7" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t>WT (Lab - BCA Lab by CHA, FHP, SG, HU, TM) in 1BCA B</t>
         </is>
       </c>
       <c r="J7" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t>WT (Lab - BCA Lab by CHA, FHP, SG, HU, TM) in 1BCA B</t>
         </is>
       </c>
     </row>
@@ -782,47 +782,47 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t>MA (Lab - BCA Lab by VKR, CYN, SG, HU, RES) in 5BCA A</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t>MA (Lab - BCA Lab by VKR, CYN, SG, HU, RES) in 5BCA A</t>
         </is>
       </c>
       <c r="G8" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="H8" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="I8" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="J8" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
     </row>
@@ -1000,12 +1000,12 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                   </t>
+          <t xml:space="preserve">PRJ (Lab - MCA Lab by BE, RV, SG, KR, VA) in 5BCA A                    </t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                   </t>
+          <t xml:space="preserve">PRJ (Lab - MCA Lab by BE, RV, SG, KR, VA) in 5BCA A                    </t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
@@ -1037,12 +1037,12 @@
       </c>
       <c r="I16" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                   </t>
+          <t xml:space="preserve">PSD (Lab - MCA Lab by AMR, SK, NEB, SME, APR) in 1BCA B                </t>
         </is>
       </c>
       <c r="J16" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                   </t>
+          <t xml:space="preserve">PSD (Lab - MCA Lab by AMR, SK, NEB, SME, APR) in 1BCA B                </t>
         </is>
       </c>
     </row>
@@ -1054,47 +1054,47 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t xml:space="preserve">WAD (Lab - MCA Lab by LJ, BE, NEB) in 3CS           </t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t xml:space="preserve">WAD (Lab - MCA Lab by LJ, BE, NEB) in 3CS           </t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t>MA (Lab - MCA Lab by VKR, CYN, SD, TM, SH) in 3BCA B</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t>MA (Lab - MCA Lab by VKR, CYN, SD, TM, SH) in 3BCA B</t>
         </is>
       </c>
       <c r="G17" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="H17" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="I17" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t xml:space="preserve">DAS (Lab - MCA Lab by SK, SME, RM, FHP, RA) in 1CM  </t>
         </is>
       </c>
       <c r="J17" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t xml:space="preserve">DAS (Lab - MCA Lab by SK, SME, RM, FHP, RA) in 1CM  </t>
         </is>
       </c>
     </row>
@@ -1106,47 +1106,47 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">DAP (Lab - MCA Lab by SME, SK, NEB, RM, SR) in 3CM  </t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">DAP (Lab - MCA Lab by SME, SK, NEB, RM, SR) in 3CM  </t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="G18" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="H18" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="I18" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t>OOP (Lab - MCA Lab by KNS, LJ, RV, SG, SA) in 1BCA B</t>
         </is>
       </c>
       <c r="J18" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t>OOP (Lab - MCA Lab by KNS, LJ, RV, SG, SA) in 1BCA B</t>
         </is>
       </c>
     </row>
@@ -1158,47 +1158,47 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">Free                                             </t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">Free                                             </t>
         </is>
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">Free                                             </t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>MA (Lab - MCA Lab by MAN) in 5BCA B</t>
+          <t xml:space="preserve">MA (Lab - MCA Lab by MAN) in 5BCA B              </t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>MA (Lab - MCA Lab by MAN) in 5BCA B</t>
+          <t xml:space="preserve">MA (Lab - MCA Lab by MAN) in 5BCA B              </t>
         </is>
       </c>
       <c r="G19" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">Free                                             </t>
         </is>
       </c>
       <c r="H19" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">Free                                             </t>
         </is>
       </c>
       <c r="I19" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t>DCF (Lab - MCA Lab by AMR, BE, MN, RV, SR) in 1CM</t>
         </is>
       </c>
       <c r="J19" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t>DCF (Lab - MCA Lab by AMR, BE, MN, RV, SR) in 1CM</t>
         </is>
       </c>
     </row>
@@ -1210,47 +1210,47 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t>MA (Lab - MCA Lab by BE, KNS, RV, NR, MAN) in 5BCA B</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t>MA (Lab - MCA Lab by BE, KNS, RV, NR, MAN) in 5BCA B</t>
         </is>
       </c>
       <c r="G20" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="H20" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="I20" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="J20" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
     </row>
@@ -1374,47 +1374,47 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>PRJ (Lab - BSc Lab by SH) in 5BCA B</t>
+          <t xml:space="preserve">PRJ (Lab - BSc Lab by SH) in 5BCA B                 </t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>PRJ (Lab - BSc Lab by SH) in 5BCA B</t>
+          <t xml:space="preserve">PRJ (Lab - BSc Lab by SH) in 5BCA B                 </t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">DAS (Lab - BSc Lab by BE, FHP, SD, RES, SH) in 1CS  </t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">DAS (Lab - BSc Lab by BE, FHP, SD, RES, SH) in 1CS  </t>
         </is>
       </c>
       <c r="G27" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="H27" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">Free                                                </t>
         </is>
       </c>
       <c r="I27" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t>WT (Lab - BSc Lab by AMR, BE, LJ, APR, KR) in 1BCA A</t>
         </is>
       </c>
       <c r="J27" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t>WT (Lab - BSc Lab by AMR, BE, LJ, APR, KR) in 1BCA A</t>
         </is>
       </c>
     </row>
@@ -1426,47 +1426,47 @@
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free   </t>
+          <t>PRJ (Lab - BSc Lab by RM, LJ, RA, HU, SH) in 5BCA B</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free   </t>
+          <t>PRJ (Lab - BSc Lab by RM, LJ, RA, HU, SH) in 5BCA B</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free   </t>
+          <t xml:space="preserve">Free                                               </t>
         </is>
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free   </t>
+          <t xml:space="preserve">Free                                               </t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free   </t>
+          <t xml:space="preserve">Free                                               </t>
         </is>
       </c>
       <c r="G28" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free   </t>
+          <t xml:space="preserve">Free                                               </t>
         </is>
       </c>
       <c r="H28" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free   </t>
+          <t xml:space="preserve">Free                                               </t>
         </is>
       </c>
       <c r="I28" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free   </t>
+          <t xml:space="preserve">Free                                               </t>
         </is>
       </c>
       <c r="J28" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free   </t>
+          <t xml:space="preserve">Free                                               </t>
         </is>
       </c>
     </row>
@@ -1478,47 +1478,47 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t xml:space="preserve">Free                                              </t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t xml:space="preserve">Free                                              </t>
         </is>
       </c>
       <c r="D29" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t xml:space="preserve">Free                                              </t>
         </is>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t xml:space="preserve">Free                                              </t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t>DA (Lab - BSc Lab by AMR, MN, RV, APR, SA) in 5CME</t>
         </is>
       </c>
       <c r="G29" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t>DA (Lab - BSc Lab by AMR, MN, RV, APR, SA) in 5CME</t>
         </is>
       </c>
       <c r="H29" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t xml:space="preserve">Free                                              </t>
         </is>
       </c>
       <c r="I29" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t xml:space="preserve">Free                                              </t>
         </is>
       </c>
       <c r="J29" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free     </t>
+          <t xml:space="preserve">Free                                              </t>
         </is>
       </c>
     </row>
@@ -1634,47 +1634,47 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                               </t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                               </t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t>WAD (Lab - BSc Lab by CHA, RM, FHP, APR, TM) in 1CM</t>
         </is>
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t>WAD (Lab - BSc Lab by CHA, RM, FHP, APR, TM) in 1CM</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">DCF (Lab - BSc Lab by RM, LJ, SR, TM, KR) in 1CS   </t>
         </is>
       </c>
       <c r="G32" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">DCF (Lab - BSc Lab by RM, LJ, SR, TM, KR) in 1CS   </t>
         </is>
       </c>
       <c r="H32" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                               </t>
         </is>
       </c>
       <c r="I32" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                               </t>
         </is>
       </c>
       <c r="J32" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free    </t>
+          <t xml:space="preserve">Free                                               </t>
         </is>
       </c>
     </row>

</xml_diff>